<commit_message>
Cleaning preprocessor script plus new data
</commit_message>
<xml_diff>
--- a/data/1-in-10-Ending-Humanity.xlsx
+++ b/data/1-in-10-Ending-Humanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/636f8a572b340079/Documents/CMU/Interactive_data_science/fp--05839-abby-jeff-kyle-will/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{21E6F362-E736-45A4-A2F6-BB30772C3C9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4265F82E-00B7-40E9-93AB-EF5D524696E9}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{21E6F362-E736-45A4-A2F6-BB30772C3C9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C91BBB91-1C15-499D-A934-157E935EA1F0}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{531A7128-E2D5-480F-8ABF-D8D7177087A7}"/>
   </bookViews>
@@ -144,9 +144,6 @@
     <t>Pursue Advancement</t>
   </si>
   <si>
-    <t xml:space="preserve">Age </t>
-  </si>
-  <si>
     <t>Gender at Birth</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>Device</t>
+  </si>
+  <si>
+    <t>Age Range</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:O402"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -539,19 +539,19 @@
         <v>35</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>

</xml_diff>